<commit_message>
Data input increased to 612, deleting unnecessary library, main model still need adjustment
</commit_message>
<xml_diff>
--- a/pooled_data.xlsx
+++ b/pooled_data.xlsx
@@ -408,7 +408,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D579"/>
+  <dimension ref="A1:D613"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -8518,6 +8518,482 @@
       </c>
       <c r="D579">
         <v>0.386</v>
+      </c>
+    </row>
+    <row r="580" spans="1:4">
+      <c r="A580">
+        <v>14.34854534416843</v>
+      </c>
+      <c r="B580">
+        <v>3.965</v>
+      </c>
+      <c r="C580">
+        <v>6.03</v>
+      </c>
+      <c r="D580">
+        <v>0.296</v>
+      </c>
+    </row>
+    <row r="581" spans="1:4">
+      <c r="A581">
+        <v>8.001250000001374</v>
+      </c>
+      <c r="B581">
+        <v>4.98</v>
+      </c>
+      <c r="C581">
+        <v>5.89</v>
+      </c>
+      <c r="D581">
+        <v>0.3181176470588235</v>
+      </c>
+    </row>
+    <row r="582" spans="1:4">
+      <c r="A582">
+        <v>5.912001383529192</v>
+      </c>
+      <c r="B582">
+        <v>4.29</v>
+      </c>
+      <c r="C582">
+        <v>5.94</v>
+      </c>
+      <c r="D582">
+        <v>0.2710999999999421</v>
+      </c>
+    </row>
+    <row r="583" spans="1:4">
+      <c r="A583">
+        <v>6.68</v>
+      </c>
+      <c r="B583">
+        <v>4.015</v>
+      </c>
+      <c r="C583">
+        <v>4.23</v>
+      </c>
+      <c r="D583">
+        <v>0.324</v>
+      </c>
+    </row>
+    <row r="584" spans="1:4">
+      <c r="A584">
+        <v>7.58</v>
+      </c>
+      <c r="B584">
+        <v>4.435</v>
+      </c>
+      <c r="C584">
+        <v>4.53</v>
+      </c>
+      <c r="D584">
+        <v>0.353206030949981</v>
+      </c>
+    </row>
+    <row r="585" spans="1:4">
+      <c r="A585">
+        <v>11.62562499999963</v>
+      </c>
+      <c r="B585">
+        <v>5.01</v>
+      </c>
+      <c r="C585">
+        <v>4.11</v>
+      </c>
+      <c r="D585">
+        <v>0.338</v>
+      </c>
+    </row>
+    <row r="586" spans="1:4">
+      <c r="A586">
+        <v>13.79999999999967</v>
+      </c>
+      <c r="B586">
+        <v>4.365</v>
+      </c>
+      <c r="C586">
+        <v>3.42</v>
+      </c>
+      <c r="D586">
+        <v>0.333</v>
+      </c>
+    </row>
+    <row r="587" spans="1:4">
+      <c r="A587">
+        <v>10.90750000000006</v>
+      </c>
+      <c r="B587">
+        <v>4.665</v>
+      </c>
+      <c r="C587">
+        <v>4.23</v>
+      </c>
+      <c r="D587">
+        <v>0.3018664137845254</v>
+      </c>
+    </row>
+    <row r="588" spans="1:4">
+      <c r="A588">
+        <v>4.52</v>
+      </c>
+      <c r="B588">
+        <v>4.005</v>
+      </c>
+      <c r="C588">
+        <v>4.56</v>
+      </c>
+      <c r="D588">
+        <v>0.2369987287018682</v>
+      </c>
+    </row>
+    <row r="589" spans="1:4">
+      <c r="A589">
+        <v>5.978823529412008</v>
+      </c>
+      <c r="B589">
+        <v>4.665</v>
+      </c>
+      <c r="C589">
+        <v>6.8</v>
+      </c>
+      <c r="D589">
+        <v>0.3371642162301796</v>
+      </c>
+    </row>
+    <row r="590" spans="1:4">
+      <c r="A590">
+        <v>4.44</v>
+      </c>
+      <c r="B590">
+        <v>4.895</v>
+      </c>
+      <c r="C590">
+        <v>6.53</v>
+      </c>
+      <c r="D590">
+        <v>0.4232575859657763</v>
+      </c>
+    </row>
+    <row r="591" spans="1:4">
+      <c r="A591">
+        <v>7.62</v>
+      </c>
+      <c r="B591">
+        <v>4.865</v>
+      </c>
+      <c r="C591">
+        <v>7.44</v>
+      </c>
+      <c r="D591">
+        <v>0.4129768452924647</v>
+      </c>
+    </row>
+    <row r="592" spans="1:4">
+      <c r="A592">
+        <v>10.67126259564734</v>
+      </c>
+      <c r="B592">
+        <v>4.83</v>
+      </c>
+      <c r="C592">
+        <v>5.13</v>
+      </c>
+      <c r="D592">
+        <v>0.3671176470588323</v>
+      </c>
+    </row>
+    <row r="593" spans="1:4">
+      <c r="A593">
+        <v>10.79812499999665</v>
+      </c>
+      <c r="B593">
+        <v>4.91</v>
+      </c>
+      <c r="C593">
+        <v>3.69</v>
+      </c>
+      <c r="D593">
+        <v>0.449</v>
+      </c>
+    </row>
+    <row r="594" spans="1:4">
+      <c r="A594">
+        <v>10.35</v>
+      </c>
+      <c r="B594">
+        <v>4.78</v>
+      </c>
+      <c r="C594">
+        <v>4.88</v>
+      </c>
+      <c r="D594">
+        <v>0.387</v>
+      </c>
+    </row>
+    <row r="595" spans="1:4">
+      <c r="A595">
+        <v>6.17</v>
+      </c>
+      <c r="B595">
+        <v>4.91</v>
+      </c>
+      <c r="C595">
+        <v>7.52</v>
+      </c>
+      <c r="D595">
+        <v>0.368</v>
+      </c>
+    </row>
+    <row r="596" spans="1:4">
+      <c r="A596">
+        <v>4.277868628312075</v>
+      </c>
+      <c r="B596">
+        <v>5.61</v>
+      </c>
+      <c r="C596">
+        <v>2.69</v>
+      </c>
+      <c r="D596">
+        <v>0.362</v>
+      </c>
+    </row>
+    <row r="597" spans="1:4">
+      <c r="A597">
+        <v>13.64687499999914</v>
+      </c>
+      <c r="B597">
+        <v>2.62</v>
+      </c>
+      <c r="C597">
+        <v>2.8</v>
+      </c>
+      <c r="D597">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="598" spans="1:4">
+      <c r="A598">
+        <v>19.79437500000008</v>
+      </c>
+      <c r="B598">
+        <v>3.09</v>
+      </c>
+      <c r="C598">
+        <v>3.14</v>
+      </c>
+      <c r="D598">
+        <v>0.325</v>
+      </c>
+    </row>
+    <row r="599" spans="1:4">
+      <c r="A599">
+        <v>6.617159854848987</v>
+      </c>
+      <c r="B599">
+        <v>4.585</v>
+      </c>
+      <c r="C599">
+        <v>5.05</v>
+      </c>
+      <c r="D599">
+        <v>0.321</v>
+      </c>
+    </row>
+    <row r="600" spans="1:4">
+      <c r="A600">
+        <v>5.11</v>
+      </c>
+      <c r="B600">
+        <v>5.115</v>
+      </c>
+      <c r="C600">
+        <v>4.1</v>
+      </c>
+      <c r="D600">
+        <v>0.3278128355862567</v>
+      </c>
+    </row>
+    <row r="601" spans="1:4">
+      <c r="A601">
+        <v>4.29</v>
+      </c>
+      <c r="B601">
+        <v>4.635</v>
+      </c>
+      <c r="C601">
+        <v>4.31</v>
+      </c>
+      <c r="D601">
+        <v>0.313</v>
+      </c>
+    </row>
+    <row r="602" spans="1:4">
+      <c r="A602">
+        <v>6.11</v>
+      </c>
+      <c r="B602">
+        <v>5.529999999999999</v>
+      </c>
+      <c r="C602">
+        <v>5.31</v>
+      </c>
+      <c r="D602">
+        <v>0.324748561669166</v>
+      </c>
+    </row>
+    <row r="603" spans="1:4">
+      <c r="A603">
+        <v>6.572336983837038</v>
+      </c>
+      <c r="B603">
+        <v>4.695</v>
+      </c>
+      <c r="C603">
+        <v>4.01</v>
+      </c>
+      <c r="D603">
+        <v>0.277</v>
+      </c>
+    </row>
+    <row r="604" spans="1:4">
+      <c r="A604">
+        <v>7.38</v>
+      </c>
+      <c r="B604">
+        <v>5.205</v>
+      </c>
+      <c r="C604">
+        <v>6.1</v>
+      </c>
+      <c r="D604">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="605" spans="1:4">
+      <c r="A605">
+        <v>12.26937499999959</v>
+      </c>
+      <c r="B605">
+        <v>11.4</v>
+      </c>
+      <c r="C605">
+        <v>2.95</v>
+      </c>
+      <c r="D605">
+        <v>0.289687824629983</v>
+      </c>
+    </row>
+    <row r="606" spans="1:4">
+      <c r="A606">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="B606">
+        <v>3.92</v>
+      </c>
+      <c r="C606">
+        <v>4.33</v>
+      </c>
+      <c r="D606">
+        <v>0.3743933793495576</v>
+      </c>
+    </row>
+    <row r="607" spans="1:4">
+      <c r="A607">
+        <v>11.43</v>
+      </c>
+      <c r="B607">
+        <v>5.085</v>
+      </c>
+      <c r="C607">
+        <v>3.15</v>
+      </c>
+      <c r="D607">
+        <v>0.371</v>
+      </c>
+    </row>
+    <row r="608" spans="1:4">
+      <c r="A608">
+        <v>14.95187500000067</v>
+      </c>
+      <c r="B608">
+        <v>4.76</v>
+      </c>
+      <c r="C608">
+        <v>3.06</v>
+      </c>
+      <c r="D608">
+        <v>0.4124117647058823</v>
+      </c>
+    </row>
+    <row r="609" spans="1:4">
+      <c r="A609">
+        <v>11.63680753643135</v>
+      </c>
+      <c r="B609">
+        <v>5.675000000000001</v>
+      </c>
+      <c r="C609">
+        <v>2.27</v>
+      </c>
+      <c r="D609">
+        <v>0.361470588235294</v>
+      </c>
+    </row>
+    <row r="610" spans="1:4">
+      <c r="A610">
+        <v>16.25602045285562</v>
+      </c>
+      <c r="B610">
+        <v>4.65</v>
+      </c>
+      <c r="C610">
+        <v>6.31</v>
+      </c>
+      <c r="D610">
+        <v>0.2826468362297734</v>
+      </c>
+    </row>
+    <row r="611" spans="1:4">
+      <c r="A611">
+        <v>6.51249994650501</v>
+      </c>
+      <c r="B611">
+        <v>21.56</v>
+      </c>
+      <c r="C611">
+        <v>4.31</v>
+      </c>
+      <c r="D611">
+        <v>0.3110614830199199</v>
+      </c>
+    </row>
+    <row r="612" spans="1:4">
+      <c r="A612">
+        <v>20.15687499999154</v>
+      </c>
+      <c r="B612">
+        <v>4.79</v>
+      </c>
+      <c r="C612">
+        <v>5.38</v>
+      </c>
+      <c r="D612">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="613" spans="1:4">
+      <c r="A613">
+        <v>26.03</v>
+      </c>
+      <c r="B613">
+        <v>9.529999999999999</v>
+      </c>
+      <c r="C613">
+        <v>2.67</v>
+      </c>
+      <c r="D613">
+        <v>0.3958235294117559</v>
       </c>
     </row>
   </sheetData>
@@ -8552,16 +9028,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>578</v>
+        <v>612</v>
       </c>
       <c r="C2">
-        <v>578</v>
+        <v>612</v>
       </c>
       <c r="D2">
-        <v>578</v>
+        <v>612</v>
       </c>
       <c r="E2">
-        <v>578</v>
+        <v>612</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -8569,16 +9045,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>10.81475778546713</v>
+        <v>10.77136470793388</v>
       </c>
       <c r="C3">
-        <v>4.499152249134949</v>
+        <v>4.553186274509804</v>
       </c>
       <c r="D3">
-        <v>5.055051903114187</v>
+        <v>5.030539215686274</v>
       </c>
       <c r="E3">
-        <v>0.3530968858131489</v>
+        <v>0.3525667678396732</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -8586,16 +9062,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>5.638554121008848</v>
+        <v>5.609864831578292</v>
       </c>
       <c r="C4">
-        <v>4.086966928357401</v>
+        <v>4.048237262985184</v>
       </c>
       <c r="D4">
-        <v>1.805692735157488</v>
+        <v>1.788318488084889</v>
       </c>
       <c r="E4">
-        <v>0.03976605273878312</v>
+        <v>0.04023879923701083</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -8620,16 +9096,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>6.3875</v>
+        <v>6.3775</v>
       </c>
       <c r="C6">
-        <v>3.32125</v>
+        <v>3.53</v>
       </c>
       <c r="D6">
-        <v>3.72</v>
+        <v>3.6975</v>
       </c>
       <c r="E6">
-        <v>0.325</v>
+        <v>0.324</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -8637,13 +9113,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>9.09</v>
+        <v>9.035</v>
       </c>
       <c r="C7">
-        <v>5.075</v>
+        <v>5.03</v>
       </c>
       <c r="D7">
-        <v>4.68</v>
+        <v>4.655</v>
       </c>
       <c r="E7">
         <v>0.351</v>
@@ -8654,16 +9130,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>13.845</v>
+        <v>13.80499999999975</v>
       </c>
       <c r="C8">
-        <v>5.77375</v>
+        <v>5.765000000000001</v>
       </c>
       <c r="D8">
-        <v>6.17</v>
+        <v>6.1625</v>
       </c>
       <c r="E8">
-        <v>0.382</v>
+        <v>0.381</v>
       </c>
     </row>
     <row r="9" spans="1:5">

</xml_diff>